<commit_message>
add phone number to file fields
</commit_message>
<xml_diff>
--- a/frontend/public/Bulk_upload_for_file_history.xlsx
+++ b/frontend/public/Bulk_upload_for_file_history.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adedapo.aderemi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dapo\FTS\web\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{152FBF91-2694-47EB-B775-8ACA2AD228F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{18759D71-B2CC-4644-86C4-4A3F49E13150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E4F42232-057A-4318-BAF7-F66AE4AE9D35}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{E4F42232-057A-4318-BAF7-F66AE4AE9D35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3" uniqueCount="3">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="4" uniqueCount="4">
   <si>
     <t>File name</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Opening date</t>
+  </si>
+  <si>
+    <t>Phone number</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D223C6BB-5ACC-4F5D-8BBA-7C312A2D9EDA}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -464,9 +467,10 @@
     <col min="1" max="1" width="17.7265625" customWidth="1"/>
     <col min="2" max="2" width="20.7265625" customWidth="1"/>
     <col min="3" max="3" width="25.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -476,28 +480,31 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>

</xml_diff>